<commit_message>
feat: complete all features and fix related issues
</commit_message>
<xml_diff>
--- a/BetaCinema.ServerUI/Template/ExportTemplates/MovieExport.xlsx
+++ b/BetaCinema.ServerUI/Template/ExportTemplates/MovieExport.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\blazor\BetaCinema\BetaCinema.ServerUI\Template\ExportTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46932D7C-2FB9-4319-90A8-96B742EC20B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5176C557-324C-4396-9646-B399C1B5DA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="DANH SÁCH PHIM" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>STT</t>
   </si>
@@ -43,10 +43,13 @@
     <t>Mô tả</t>
   </si>
   <si>
+    <t>Ngày khởi chiếu</t>
+  </si>
+  <si>
+    <t>Thể loại</t>
+  </si>
+  <si>
     <t>Thời lượng</t>
-  </si>
-  <si>
-    <t>Ngày khởi chiếu</t>
   </si>
 </sst>
 </file>
@@ -121,11 +124,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -133,14 +133,22 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -459,74 +467,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B78FB58-FC69-45B8-BE8C-0DCDA3C69853}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.21875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="50.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="43.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.77734375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="36.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="60.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.21875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="22.77734375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="38.33203125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="80.6640625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="17.21875" style="8" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+    <row r="4" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>1</v>
       </c>
       <c r="B4" s="4"/>
@@ -536,11 +551,12 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
   </mergeCells>
   <pageMargins left="0.39370078740157477" right="0.39370078740157477" top="0.39370078740157477" bottom="0.39370078740157477" header="0.5" footer="0.5"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>

</xml_diff>